<commit_message>
Atualização do backlog (adicionados RF31 ao RF34)
</commit_message>
<xml_diff>
--- a/private/backlog/Backlog_projeto-individual.xlsx
+++ b/private/backlog/Backlog_projeto-individual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\projetoNeedForSpeed\private\backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D31554C-980D-4702-875C-237EA927B764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1807F8-7AF2-49EF-8DD3-953531AACBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BEB80C7E-25DF-4BD2-BFDC-80B8AEDF43D5}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="11520" xr2:uid="{BEB80C7E-25DF-4BD2-BFDC-80B8AEDF43D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog Projeto Individual" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="98">
   <si>
     <t>Classificação</t>
   </si>
@@ -283,6 +283,42 @@
   </si>
   <si>
     <t>Desejável</t>
+  </si>
+  <si>
+    <t>RF31</t>
+  </si>
+  <si>
+    <t>RF32</t>
+  </si>
+  <si>
+    <t>RF33</t>
+  </si>
+  <si>
+    <t>RF34</t>
+  </si>
+  <si>
+    <t>Diagrama de Visão de Negócio</t>
+  </si>
+  <si>
+    <t>Criar e adicionar como parte da documentação</t>
+  </si>
+  <si>
+    <t>Sequencia de Fibonacci</t>
+  </si>
+  <si>
+    <t>Adicionar ao backlog, para criar o gráfico de Burndown</t>
+  </si>
+  <si>
+    <t>Gráfico de Burndown</t>
+  </si>
+  <si>
+    <t>Incluir ao backlog do produto</t>
+  </si>
+  <si>
+    <t>Service Level Agreement do projeto</t>
+  </si>
+  <si>
+    <t>Criar o SLA -  responsabilidade entre cliente e provedor</t>
   </si>
 </sst>
 </file>
@@ -707,10 +743,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DCD705-25E0-43CC-9266-7D636D99DF43}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1156,6 +1192,62 @@
         <v>85</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>